<commit_message>
Add some sprites and update dialogform
添加一些UI资源，更新弹出对话框的功能。
</commit_message>
<xml_diff>
--- a/Common/Excel/UIForm.xlsx
+++ b/Common/Excel/UIForm.xlsx
@@ -468,7 +468,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -564,7 +564,7 @@
         <v>1</v>
       </c>
       <c r="F5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>